<commit_message>
upload classification 89: native model regions.
</commit_message>
<xml_diff>
--- a/IEDC_queries/IEDC_advanced_search_lookupvalues_vMarch2025.xlsx
+++ b/IEDC_queries/IEDC_advanced_search_lookupvalues_vMarch2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Pauliuk\FILES\ARBEIT\PROJECTS\Database\IE_DataCommons\IEDC_software\IEDC_queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7472AAF3-5520-49A9-957A-BBFF8A8BDE16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D6D07F-1BF2-4E56-9E89-5C3A1C59C249}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20922" windowHeight="9372" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5871" uniqueCount="5650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5970" uniqueCount="5686">
   <si>
     <t>Dropdown labels</t>
   </si>
@@ -16970,6 +16970,114 @@
   </si>
   <si>
     <t>Aspect id</t>
+  </si>
+  <si>
+    <t>Criticality indicators (6_CR) by material (4011 entries)</t>
+  </si>
+  <si>
+    <t>Labels_15</t>
+  </si>
+  <si>
+    <t>AgInCd alloy</t>
+  </si>
+  <si>
+    <t>AISI 410</t>
+  </si>
+  <si>
+    <t>AISI 430</t>
+  </si>
+  <si>
+    <t>AISI 444</t>
+  </si>
+  <si>
+    <t>Alumina</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>CaO</t>
+  </si>
+  <si>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>Ceramic composite</t>
+  </si>
+  <si>
+    <t>Chromite</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Crude oil</t>
+  </si>
+  <si>
+    <t>Epoxy</t>
+  </si>
+  <si>
+    <t>Fluorspar</t>
+  </si>
+  <si>
+    <t>FRP</t>
+  </si>
+  <si>
+    <t>GaIn Alloy</t>
+  </si>
+  <si>
+    <t>Galinstan</t>
+  </si>
+  <si>
+    <t>HSS T1</t>
+  </si>
+  <si>
+    <t>Iron oxide</t>
+  </si>
+  <si>
+    <t>Lithium Battery Mix</t>
+  </si>
+  <si>
+    <t>Membrane</t>
+  </si>
+  <si>
+    <t>MgAl2O4</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>NaCl</t>
+  </si>
+  <si>
+    <t>Natural gas</t>
+  </si>
+  <si>
+    <t>Nitrogen</t>
+  </si>
+  <si>
+    <t>PET</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>SO2</t>
+  </si>
+  <si>
+    <t>Stainless steel</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Talc</t>
+  </si>
+  <si>
+    <t>Wood</t>
   </si>
 </sst>
 </file>
@@ -17324,10 +17432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4215"/>
+  <dimension ref="A1:S4215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -17337,7 +17445,7 @@
     <col min="3" max="3" width="21.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17392,8 +17500,11 @@
       <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S1" s="1" t="s">
+        <v>5651</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -17448,8 +17559,11 @@
       <c r="R2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -17504,8 +17618,11 @@
       <c r="R3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S3" t="s">
+        <v>5652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -17560,8 +17677,11 @@
       <c r="R4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S4" t="s">
+        <v>5653</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -17616,8 +17736,11 @@
       <c r="R5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S5" t="s">
+        <v>5654</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -17672,8 +17795,11 @@
       <c r="R6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S6" t="s">
+        <v>5655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -17728,8 +17854,11 @@
       <c r="R7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -17784,8 +17913,11 @@
       <c r="R8" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S8" t="s">
+        <v>5656</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -17840,8 +17972,11 @@
       <c r="R9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -17896,8 +18031,11 @@
       <c r="R10" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -17952,8 +18090,11 @@
       <c r="R11" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>159</v>
       </c>
@@ -18005,8 +18146,11 @@
       <c r="R12" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>172</v>
       </c>
@@ -18058,8 +18202,11 @@
       <c r="R13" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>184</v>
       </c>
@@ -18108,8 +18255,11 @@
       <c r="R14" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>195</v>
       </c>
@@ -18158,8 +18308,11 @@
       <c r="R15" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S15" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>207</v>
       </c>
@@ -18208,8 +18361,20 @@
       <c r="R16" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S16" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>5650</v>
+      </c>
+      <c r="B17">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>26</v>
+      </c>
       <c r="D17" t="s">
         <v>219</v>
       </c>
@@ -18249,8 +18414,11 @@
       <c r="R17" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D18" t="s">
         <v>221</v>
       </c>
@@ -18290,8 +18458,11 @@
       <c r="R18" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D19" t="s">
         <v>85</v>
       </c>
@@ -18331,8 +18502,11 @@
       <c r="R19" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S19" t="s">
+        <v>5659</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D20" t="s">
         <v>252</v>
       </c>
@@ -18372,8 +18546,11 @@
       <c r="R20" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S20" t="s">
+        <v>5660</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D21" t="s">
         <v>241</v>
       </c>
@@ -18413,8 +18590,11 @@
       <c r="R21" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S21" t="s">
+        <v>5661</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D22" t="s">
         <v>276</v>
       </c>
@@ -18454,8 +18634,11 @@
       <c r="R22" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="23" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S22" t="s">
+        <v>5662</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D23" t="s">
         <v>288</v>
       </c>
@@ -18495,8 +18678,11 @@
       <c r="R23" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="24" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D24" t="s">
         <v>299</v>
       </c>
@@ -18536,8 +18722,11 @@
       <c r="R24" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="25" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S24" t="s">
+        <v>5663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" t="s">
         <v>311</v>
       </c>
@@ -18577,8 +18766,11 @@
       <c r="R25" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="26" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" t="s">
         <v>322</v>
       </c>
@@ -18612,8 +18804,11 @@
       <c r="R26" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S26" t="s">
+        <v>5664</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D27" t="s">
         <v>331</v>
       </c>
@@ -18647,8 +18842,11 @@
       <c r="R27" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D28" t="s">
         <v>333</v>
       </c>
@@ -18682,8 +18880,11 @@
       <c r="R28" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="29" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S28" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D29" t="s">
         <v>352</v>
       </c>
@@ -18717,8 +18918,11 @@
       <c r="R29" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="30" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S29" t="s">
+        <v>5665</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D30" t="s">
         <v>343</v>
       </c>
@@ -18752,8 +18956,11 @@
       <c r="R30" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="31" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D31" t="s">
         <v>372</v>
       </c>
@@ -18787,8 +18994,11 @@
       <c r="R31" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="32" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S31" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D32" t="s">
         <v>382</v>
       </c>
@@ -18822,8 +19032,11 @@
       <c r="R32" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="33" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D33" t="s">
         <v>374</v>
       </c>
@@ -18854,8 +19067,11 @@
       <c r="R33" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="34" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S33" t="s">
+        <v>5666</v>
+      </c>
+    </row>
+    <row r="34" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D34" t="s">
         <v>401</v>
       </c>
@@ -18886,8 +19102,11 @@
       <c r="R34" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="35" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S34" t="s">
+        <v>5667</v>
+      </c>
+    </row>
+    <row r="35" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="D35" t="s">
         <v>384</v>
       </c>
@@ -18918,8 +19137,11 @@
       <c r="R35" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="36" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S35" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E36" t="s">
         <v>417</v>
       </c>
@@ -18947,8 +19169,11 @@
       <c r="R36" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="37" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S36" t="s">
+        <v>5668</v>
+      </c>
+    </row>
+    <row r="37" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E37" t="s">
         <v>426</v>
       </c>
@@ -18976,8 +19201,11 @@
       <c r="R37" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S37" t="s">
+        <v>5669</v>
+      </c>
+    </row>
+    <row r="38" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E38" t="s">
         <v>434</v>
       </c>
@@ -19005,8 +19233,11 @@
       <c r="R38" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="39" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E39" t="s">
         <v>443</v>
       </c>
@@ -19034,8 +19265,11 @@
       <c r="R39" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="40" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S39" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="40" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E40" t="s">
         <v>452</v>
       </c>
@@ -19063,8 +19297,11 @@
       <c r="R40" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="41" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="41" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E41" t="s">
         <v>460</v>
       </c>
@@ -19092,8 +19329,11 @@
       <c r="R41" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="42" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E42" t="s">
         <v>176</v>
       </c>
@@ -19121,8 +19361,11 @@
       <c r="R42" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="43" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S42" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="43" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E43" t="s">
         <v>477</v>
       </c>
@@ -19150,8 +19393,11 @@
       <c r="R43" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="44" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S43" t="s">
+        <v>5670</v>
+      </c>
+    </row>
+    <row r="44" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E44" t="s">
         <v>486</v>
       </c>
@@ -19179,8 +19425,11 @@
       <c r="R44" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="45" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S44" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="45" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E45" t="s">
         <v>495</v>
       </c>
@@ -19208,8 +19457,11 @@
       <c r="R45" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="46" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S45" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="46" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E46" t="s">
         <v>504</v>
       </c>
@@ -19237,8 +19489,11 @@
       <c r="R46" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="47" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S46" t="s">
+        <v>5671</v>
+      </c>
+    </row>
+    <row r="47" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E47" t="s">
         <v>512</v>
       </c>
@@ -19266,8 +19521,11 @@
       <c r="R47" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="48" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="48" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" t="s">
         <v>520</v>
       </c>
@@ -19295,8 +19553,11 @@
       <c r="R48" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="49" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S48" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="49" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E49" t="s">
         <v>529</v>
       </c>
@@ -19324,8 +19585,11 @@
       <c r="R49" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="50" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S49" t="s">
+        <v>5672</v>
+      </c>
+    </row>
+    <row r="50" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E50" t="s">
         <v>537</v>
       </c>
@@ -19353,8 +19617,11 @@
       <c r="R50" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="51" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S50" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="51" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E51" t="s">
         <v>545</v>
       </c>
@@ -19382,8 +19649,11 @@
       <c r="R51" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="52" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S51" t="s">
+        <v>5673</v>
+      </c>
+    </row>
+    <row r="52" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E52" t="s">
         <v>553</v>
       </c>
@@ -19411,8 +19681,11 @@
       <c r="R52" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="53" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S52" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="53" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E53" t="s">
         <v>562</v>
       </c>
@@ -19440,8 +19713,11 @@
       <c r="R53" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="54" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S53" t="s">
+        <v>5674</v>
+      </c>
+    </row>
+    <row r="54" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E54" t="s">
         <v>570</v>
       </c>
@@ -19469,8 +19745,11 @@
       <c r="R54" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="55" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S54" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="55" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E55" t="s">
         <v>579</v>
       </c>
@@ -19498,8 +19777,11 @@
       <c r="R55" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="56" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S55" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E56" t="s">
         <v>63</v>
       </c>
@@ -19527,8 +19809,11 @@
       <c r="R56" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="57" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S56" t="s">
+        <v>5675</v>
+      </c>
+    </row>
+    <row r="57" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E57" t="s">
         <v>594</v>
       </c>
@@ -19556,8 +19841,11 @@
       <c r="R57" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="58" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S57" t="s">
+        <v>5676</v>
+      </c>
+    </row>
+    <row r="58" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E58" t="s">
         <v>603</v>
       </c>
@@ -19585,8 +19873,11 @@
       <c r="R58" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="59" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S58" t="s">
+        <v>5677</v>
+      </c>
+    </row>
+    <row r="59" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E59" t="s">
         <v>611</v>
       </c>
@@ -19614,8 +19905,11 @@
       <c r="R59" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="60" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S59" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="60" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E60" t="s">
         <v>619</v>
       </c>
@@ -19643,8 +19937,11 @@
       <c r="R60" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="61" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S60" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="61" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E61" t="s">
         <v>628</v>
       </c>
@@ -19672,8 +19969,11 @@
       <c r="R61" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="62" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S61" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="62" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E62" t="s">
         <v>637</v>
       </c>
@@ -19701,8 +20001,11 @@
       <c r="R62" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="63" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S62" t="s">
+        <v>5678</v>
+      </c>
+    </row>
+    <row r="63" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E63" t="s">
         <v>646</v>
       </c>
@@ -19727,8 +20030,11 @@
       <c r="R63" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="64" spans="5:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S63" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="64" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E64" t="s">
         <v>653</v>
       </c>
@@ -19750,8 +20056,11 @@
       <c r="Q64" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="65" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S64" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="65" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E65" t="s">
         <v>660</v>
       </c>
@@ -19770,8 +20079,11 @@
       <c r="Q65" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="66" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="66" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E66" t="s">
         <v>666</v>
       </c>
@@ -19790,8 +20102,11 @@
       <c r="Q66" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="67" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S66" t="s">
+        <v>5679</v>
+      </c>
+    </row>
+    <row r="67" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E67" t="s">
         <v>672</v>
       </c>
@@ -19810,8 +20125,11 @@
       <c r="Q67" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="68" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S67" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="68" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E68" t="s">
         <v>677</v>
       </c>
@@ -19830,8 +20148,11 @@
       <c r="Q68" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="69" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S68" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="69" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E69" t="s">
         <v>682</v>
       </c>
@@ -19850,8 +20171,11 @@
       <c r="Q69" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="70" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S69" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="70" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E70" t="s">
         <v>688</v>
       </c>
@@ -19870,8 +20194,11 @@
       <c r="Q70" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="71" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S70" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="71" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E71" t="s">
         <v>694</v>
       </c>
@@ -19890,8 +20217,11 @@
       <c r="Q71" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="72" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S71" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="72" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E72" t="s">
         <v>699</v>
       </c>
@@ -19910,8 +20240,11 @@
       <c r="Q72" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="73" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S72" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="73" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E73" t="s">
         <v>704</v>
       </c>
@@ -19930,8 +20263,11 @@
       <c r="Q73" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="74" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S73" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="74" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E74" t="s">
         <v>709</v>
       </c>
@@ -19950,8 +20286,11 @@
       <c r="Q74" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="75" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S74" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="75" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E75" t="s">
         <v>714</v>
       </c>
@@ -19970,8 +20309,11 @@
       <c r="Q75" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="76" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S75" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="76" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E76" t="s">
         <v>719</v>
       </c>
@@ -19990,8 +20332,11 @@
       <c r="Q76" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="77" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S76" t="s">
+        <v>5680</v>
+      </c>
+    </row>
+    <row r="77" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E77" t="s">
         <v>723</v>
       </c>
@@ -20010,8 +20355,11 @@
       <c r="Q77" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="78" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S77" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="78" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E78" t="s">
         <v>727</v>
       </c>
@@ -20030,8 +20378,11 @@
       <c r="Q78" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="79" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S78" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="79" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E79" t="s">
         <v>733</v>
       </c>
@@ -20050,8 +20401,11 @@
       <c r="Q79" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="80" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S79" t="s">
+        <v>5681</v>
+      </c>
+    </row>
+    <row r="80" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E80" t="s">
         <v>738</v>
       </c>
@@ -20070,8 +20424,11 @@
       <c r="Q80" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="81" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S80" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="81" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E81" t="s">
         <v>744</v>
       </c>
@@ -20090,8 +20447,11 @@
       <c r="Q81" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="82" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S81" t="s">
+        <v>5682</v>
+      </c>
+    </row>
+    <row r="82" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E82" t="s">
         <v>749</v>
       </c>
@@ -20110,8 +20470,11 @@
       <c r="Q82" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="83" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S82" t="s">
+        <v>5683</v>
+      </c>
+    </row>
+    <row r="83" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E83" t="s">
         <v>755</v>
       </c>
@@ -20127,8 +20490,11 @@
       <c r="K83" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="84" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S83" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="84" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E84" t="s">
         <v>759</v>
       </c>
@@ -20144,8 +20510,11 @@
       <c r="K84" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="85" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S84" t="s">
+        <v>5684</v>
+      </c>
+    </row>
+    <row r="85" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E85" t="s">
         <v>764</v>
       </c>
@@ -20161,8 +20530,11 @@
       <c r="K85" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="86" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S85" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="86" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E86" t="s">
         <v>769</v>
       </c>
@@ -20178,8 +20550,11 @@
       <c r="K86" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="87" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S86" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="87" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E87" t="s">
         <v>773</v>
       </c>
@@ -20195,8 +20570,11 @@
       <c r="K87" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="88" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S87" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="88" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E88" t="s">
         <v>777</v>
       </c>
@@ -20212,8 +20590,11 @@
       <c r="K88" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="89" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S88" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="89" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E89" t="s">
         <v>781</v>
       </c>
@@ -20229,8 +20610,11 @@
       <c r="K89" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="90" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S89" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="90" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E90" t="s">
         <v>785</v>
       </c>
@@ -20246,8 +20630,11 @@
       <c r="K90" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="91" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S90" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="91" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E91" t="s">
         <v>790</v>
       </c>
@@ -20263,8 +20650,11 @@
       <c r="K91" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="92" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S91" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="92" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E92" t="s">
         <v>795</v>
       </c>
@@ -20280,8 +20670,11 @@
       <c r="K92" t="s">
         <v>798</v>
       </c>
-    </row>
-    <row r="93" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S92" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="93" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E93" t="s">
         <v>93</v>
       </c>
@@ -20297,8 +20690,11 @@
       <c r="K93" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="94" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S93" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="94" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E94" t="s">
         <v>802</v>
       </c>
@@ -20314,8 +20710,11 @@
       <c r="K94" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="95" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S94" t="s">
+        <v>5685</v>
+      </c>
+    </row>
+    <row r="95" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E95" t="s">
         <v>807</v>
       </c>
@@ -20331,8 +20730,11 @@
       <c r="K95" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="96" spans="5:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="S95" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="96" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E96" t="s">
         <v>812</v>
       </c>
@@ -20348,8 +20750,11 @@
       <c r="K96" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="97" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="S96" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="97" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E97" t="s">
         <v>816</v>
       </c>
@@ -20365,8 +20770,11 @@
       <c r="K97" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="98" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="S97" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="98" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E98" t="s">
         <v>820</v>
       </c>
@@ -20382,8 +20790,11 @@
       <c r="K98" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="99" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="S98" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="99" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E99" t="s">
         <v>825</v>
       </c>
@@ -20400,7 +20811,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="100" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E100" t="s">
         <v>830</v>
       </c>
@@ -20417,7 +20828,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="101" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E101" t="s">
         <v>835</v>
       </c>
@@ -20434,7 +20845,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="102" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E102" t="s">
         <v>840</v>
       </c>
@@ -20451,7 +20862,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="103" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E103" t="s">
         <v>845</v>
       </c>
@@ -20468,7 +20879,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="104" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E104" t="s">
         <v>850</v>
       </c>
@@ -20485,7 +20896,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="105" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E105" t="s">
         <v>854</v>
       </c>
@@ -20502,7 +20913,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="106" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E106" t="s">
         <v>858</v>
       </c>
@@ -20519,7 +20930,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="107" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E107" t="s">
         <v>863</v>
       </c>
@@ -20536,7 +20947,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="108" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E108" t="s">
         <v>867</v>
       </c>
@@ -20553,7 +20964,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="109" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E109" t="s">
         <v>872</v>
       </c>
@@ -20570,7 +20981,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="110" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E110" t="s">
         <v>876</v>
       </c>
@@ -20587,7 +20998,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="111" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E111" t="s">
         <v>881</v>
       </c>
@@ -20604,7 +21015,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="112" spans="5:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="5:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E112" t="s">
         <v>885</v>
       </c>
@@ -21941,7 +22352,7 @@
     </row>
     <row r="208" spans="5:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E208" t="s">
-        <v>1252</v>
+        <v>1255</v>
       </c>
       <c r="H208" t="s">
         <v>1253</v>
@@ -21952,7 +22363,7 @@
     </row>
     <row r="209" spans="5:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E209" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="H209" t="s">
         <v>1256</v>
@@ -24083,7 +24494,7 @@
     </row>
     <row r="436" spans="5:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E436" t="s">
-        <v>113</v>
+        <v>1806</v>
       </c>
       <c r="K436" t="s">
         <v>1805</v>
@@ -24091,7 +24502,7 @@
     </row>
     <row r="437" spans="5:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E437" t="s">
-        <v>1806</v>
+        <v>113</v>
       </c>
       <c r="K437" t="s">
         <v>1807</v>

</xml_diff>